<commit_message>
update index and bash
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>linux</t>
   </si>
@@ -57,72 +57,209 @@
   </si>
   <si>
     <t>How to make a batch file</t>
+  </si>
+  <si>
+    <t>Delete a folder with all its content</t>
+  </si>
+  <si>
+    <t>Change Read-only to Editable</t>
+  </si>
+  <si>
+    <t>About Environment Variable:</t>
+  </si>
+  <si>
+    <t>Unzip a tar file</t>
+  </si>
+  <si>
+    <t>History command</t>
+  </si>
+  <si>
+    <t>$ history
+$ ! n (n is the history command no.)</t>
+  </si>
+  <si>
+    <t>Grep command</t>
+  </si>
+  <si>
+    <t>$ history | grep {searchparameter}</t>
+  </si>
+  <si>
+    <t>Piping command</t>
+  </si>
+  <si>
+    <t>$ echo "String to be writen" &gt; /etc/{some document}</t>
+  </si>
+  <si>
+    <t>TOPIC</t>
+  </si>
+  <si>
+    <t>DSCP</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>install git</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>apt-get install git-all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linux</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>install unity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>apt-get install ubuntu-desktop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>apt-get install vnc4server</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vncsever</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ sudo tar -xf {file.tar.gz} -C {target direcotry}
+$ sudo tar zxvf {filename} 
+-x extract
+-f </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">指明後面的參數是文件名
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-C change result to follow path
+-z </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>指明是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>tar.gz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">類型
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-v verbolsely state process</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/*set*/ JAVA_HOME=~/jdk
+/*export*/ export JAVA_HOME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>variable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$ set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>會顯示所有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Environment variable
+$ printenv MAVEN_HOME </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>等價於</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> echo $MAVEN_HOME</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1. nano a *.sh file
 2. insert header #!/bin/bash and your command below
 3. chmod +x *.sh
 4. $./*.sh</t>
-  </si>
-  <si>
-    <t>Delete a folder with all its content</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$sudo chmod u+w {target_file}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>$sudo rm -R {target_folder}</t>
-  </si>
-  <si>
-    <t>Change Read-only to Editable</t>
-  </si>
-  <si>
-    <t>$sudo chmod u+w {target_file}</t>
-  </si>
-  <si>
-    <t>About Environment Variable:</t>
-  </si>
-  <si>
-    <t>$ set 會顯示所有Environment variable
-$ printenv MAVEN_HOME 等價於 echo $MAVEN_HOME</t>
-  </si>
-  <si>
-    <t>Unzip a tar file</t>
-  </si>
-  <si>
-    <t>$ sudo tar -xf {file.tar.gz} -C {target direcotry}</t>
-  </si>
-  <si>
-    <t>History command</t>
-  </si>
-  <si>
-    <t>$ history
-$ ! n (n is the history command no.)</t>
-  </si>
-  <si>
-    <t>Grep command</t>
-  </si>
-  <si>
-    <t>$ history | grep {searchparameter}</t>
-  </si>
-  <si>
-    <t>Piping command</t>
-  </si>
-  <si>
-    <t>$ echo "String to be writen" &gt; /etc/{some document}</t>
-  </si>
-  <si>
-    <t>TOPIC</t>
-  </si>
-  <si>
-    <t>DSCP</t>
-  </si>
-  <si>
-    <t>CODE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +285,12 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -487,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -502,13 +645,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -566,15 +709,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -582,10 +725,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -593,32 +736,32 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="93" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,10 +769,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,11 +791,60 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
pentest, linux cpu info, andriod studio
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>linux</t>
   </si>
@@ -382,6 +382,18 @@
   </si>
   <si>
     <t xml:space="preserve">In linux, there is a script call .bashrc in your ~ directory that run on your boot. You can export your env variable in this script. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check cpu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat /proc/cpuinfo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -767,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1098,17 @@
       </c>
       <c r="C28" s="2" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add nmap entry to bash_lib
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>linux</t>
   </si>
@@ -272,16 +272,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>udp: echo "foobar" | nc -u -w1 localhost 5000
-tcp: echo "foobar" | nc 127.0.0.1 5000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>udp: nc -lu localhost 5000
-tcp: nc -l 5000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>tcp: nc -vnz -w 1 192.168.233.208 1-1000 2000-3000
 udp: nc -vnzu 192.168.1.8 1-65535</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -395,17 +385,37 @@
   <si>
     <t>linux</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>udp: echo "foobar" | nc -u -w1 localhost 5000
+tcp: echo "foobar" | nc 127.0.0.1 5000</t>
+  </si>
+  <si>
+    <t>udp: nc -lu localhost 5000
+tcp: nc -l 5000</t>
+  </si>
+  <si>
+    <t>Nmap</t>
+  </si>
+  <si>
+    <t>scan target</t>
+  </si>
+  <si>
+    <t>The format of nmap is: $nmap [Scan types] [Options] {target_ip_address}
+$namp -sS 127.0.0.1
+$nmap -sS 127.*.*.1-255
+$nmap -sX -p 20,30,40,8080 127.0.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -416,7 +426,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -480,7 +490,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -493,7 +503,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -567,7 +577,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -602,7 +611,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -778,21 +786,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" customWidth="1"/>
     <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="56.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -803,7 +811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="26.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -811,10 +819,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -825,7 +833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -836,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -847,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -855,10 +863,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51.75">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -869,7 +877,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="26.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -880,7 +888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="26.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -891,7 +899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -899,10 +907,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="93" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="93">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -913,7 +921,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -924,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -935,7 +943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -946,7 +954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -957,7 +965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -968,7 +976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -979,7 +987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="26.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -987,10 +995,10 @@
         <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="27" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="27">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1001,7 +1009,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1009,10 +1017,10 @@
         <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1023,7 +1031,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1031,10 +1039,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1042,10 +1050,10 @@
         <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="26.25">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1053,62 +1061,73 @@
         <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="39">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="26.25">
       <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>64</v>
+    <row r="30" spans="1:3" ht="51.75">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1119,12 +1138,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1132,12 +1151,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add sed usage example and cmd ren entry
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>linux</t>
   </si>
@@ -405,6 +405,25 @@
 $namp -sS 127.0.0.1
 $nmap -sS 127.*.*.1-255
 $nmap -sX -p 20,30,40,8080 127.0.0.1</t>
+  </si>
+  <si>
+    <t>Sed</t>
+  </si>
+  <si>
+    <t>basic ops</t>
+  </si>
+  <si>
+    <t>Delete lines:
+&gt; sed '/^u/d' input.txt              //delete lines start with char 'u'</t>
+  </si>
+  <si>
+    <t>for + sed</t>
+  </si>
+  <si>
+    <t>Clear all comment and save java source to a file with suffix 'Cleaned'</t>
+  </si>
+  <si>
+    <t>for f in $(find *.java -type f); do sed '/*/d' $f &gt; ${f}.Cleaned.java; done</t>
   </si>
 </sst>
 </file>
@@ -480,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -488,6 +507,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1128,6 +1150,28 @@
       </c>
       <c r="C30" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="31.5">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update bash.lib entry about find usage
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -359,10 +359,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>$find {search-path} -name "*.pdf"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>linux</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -425,16 +421,41 @@
   <si>
     <t>for f in $(find *.java -type f); do sed '/*/d' $f &gt; ${f}.Cleaned.java; done</t>
   </si>
+  <si>
+    <r>
+      <t>$find {search-path} -name "*.pdf"
+$find (search-path} -type f              //</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">指定查找文件類型文件
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>p.s. default search into sub-directories.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -445,7 +466,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -512,7 +533,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -525,7 +546,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -599,6 +620,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -633,6 +655,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,21 +831,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="56.375" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -833,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25">
+    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +867,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -855,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -866,7 +889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -877,7 +900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -885,10 +908,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="51.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -899,7 +922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25">
+    <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -910,7 +933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="26.25">
+    <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -921,7 +944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5">
+    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -932,7 +955,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="93">
+    <row r="11" spans="1:3" ht="94.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -943,7 +966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -954,7 +977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -965,7 +988,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -976,7 +999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -987,7 +1010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -998,7 +1021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1009,7 +1032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26.25">
+    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1020,7 +1043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27">
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1031,7 +1054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1042,7 +1065,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1053,7 +1076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="26.25">
+    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1061,10 +1084,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="26.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1072,10 +1095,10 @@
         <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="26.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1086,7 +1109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="26.25">
+    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1097,7 +1120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="39">
+    <row r="26" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -1108,7 +1131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1119,59 +1142,59 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25">
+    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="51.75">
+    </row>
+    <row r="30" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="31.5">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>73</v>
-      </c>
-      <c r="C32" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1182,12 +1205,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1195,12 +1218,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add bash on how to run cmd background
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>linux</t>
   </si>
@@ -446,16 +446,30 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>run a cmd at background</t>
+  </si>
+  <si>
+    <t>Run a cmd at background:
+&gt; {command_body} &amp;
+Check the process:
+&gt; top
+&gt; ps -a
+&gt; pstree</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -466,7 +480,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -533,7 +547,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -546,7 +560,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,7 +634,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -655,7 +668,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -831,21 +843,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="56.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -856,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="26.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +879,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -878,7 +890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -889,7 +901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -900,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="40.5">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -911,7 +923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="51.75">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -922,7 +934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="26.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="26.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -944,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -955,7 +967,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="94.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="93">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -966,7 +978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -977,7 +989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -988,7 +1000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1021,7 +1033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1032,7 +1044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="26.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="27">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1054,7 +1066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1087,7 +1099,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="26.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="26.25">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1120,7 +1132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="39">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -1153,7 +1165,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="51.75">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -1175,7 +1187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="31.5">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1195,6 +1207,17 @@
       </c>
       <c r="C32" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="94.5">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1205,12 +1228,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,12 +1241,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add bash entry about ICONV and XXD. Both of them are related to doc encoding.
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>linux</t>
   </si>
@@ -459,6 +459,20 @@
 &gt; top
 &gt; ps -a
 &gt; pstree</t>
+  </si>
+  <si>
+    <t>Encode</t>
+  </si>
+  <si>
+    <t>Introduce ICONV to convert encoding and XXD to cat in HEX</t>
+  </si>
+  <si>
+    <t>Convert from file a to file b: 
+&gt; iconv -f ASCII -t UTF-8 &lt; fileA.txt &gt; fileB.txt
+Show the encoding option:
+&gt; iconv -l 
+Show HEX of a file:
+&gt; xxd filea.txt</t>
   </si>
 </sst>
 </file>
@@ -844,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1218,6 +1232,17 @@
       </c>
       <c r="C33" s="5" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="94.5">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add bash entry on Tar usage
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>linux</t>
   </si>
@@ -474,12 +474,101 @@
 Show HEX of a file:
 &gt; xxd filea.txt</t>
   </si>
+  <si>
+    <t>Tar</t>
+  </si>
+  <si>
+    <t>$ tar cvf wallpaper.tar WallPaper    //package all content in WallPaper folder
+$ tar tf wallpaper.tar  //display content in pack
+$ tar xvf wallpaper.tar   //extract pack</t>
+  </si>
+  <si>
+    <t>Package option</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>create a package: cvf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+c–create create a new archive
+v–verbose verbosely list files processed
+f–file=ARCHIVE use archive file or device ARCHIVE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>display the content: tf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+t–list list the contents of an archive
+f–file=ARCHIVE use archive file or device ARCHIVE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extract the package: xvf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+x–extract, –get extract files from an archive
+v–verbose verbosely list files processed
+f–file=ARCHIVE use archive file or device ARCHIVE</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +600,14 @@
       <name val="細明體"/>
       <family val="3"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -858,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1243,6 +1340,28 @@
       </c>
       <c r="C34" s="5" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="63">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="173.25">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some sommon use reference to Java, and add find util regex to bash entries
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>linux</t>
   </si>
@@ -562,6 +562,17 @@
 v–verbose verbosely list files processed
 f–file=ARCHIVE use archive file or device ARCHIVE</t>
     </r>
+  </si>
+  <si>
+    <t>Find</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>$ find -regex ".*ABC.*"
+1. option -iregex is for non capital sensitive 
+2. Notice that it’s a path match but not a search (the  -name option for example is a search)</t>
   </si>
 </sst>
 </file>
@@ -955,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1362,6 +1373,17 @@
       </c>
       <c r="C36" s="5" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="63">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add bash entry about pushd/popd/dirs, sed replace and a case
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>linux</t>
   </si>
@@ -573,6 +573,37 @@
     <t>$ find -regex ".*ABC.*"
 1. option -iregex is for non capital sensitive 
 2. Notice that it’s a path match but not a search (the  -name option for example is a search)</t>
+  </si>
+  <si>
+    <t>pushd/popd</t>
+  </si>
+  <si>
+    <t>sed</t>
+  </si>
+  <si>
+    <t>echo $PATH | sed s/:/\\n/g</t>
+  </si>
+  <si>
+    <t>replace : character with \n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basic </t>
+  </si>
+  <si>
+    <t>pushd {path} //perform cd and push the path to stack
+popd {path} //pop the stack and cd to the poped path
+dirs //show your DIRectory Stack</t>
+  </si>
+  <si>
+    <t>案例</t>
+  </si>
+  <si>
+    <t>找出bash在call哪個vim</t>
+  </si>
+  <si>
+    <t>for f in $(echo $PATH | sed s/:/\\n/g);
+    do find $f -name "vim.exe";
+done</t>
   </si>
 </sst>
 </file>
@@ -966,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1384,6 +1415,39 @@
       </c>
       <c r="C37" s="5" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="47.25">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="47.25">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add bash entry on cut
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>linux</t>
   </si>
@@ -604,6 +604,23 @@
     <t>for f in $(echo $PATH | sed s/:/\\n/g);
     do find $f -name "vim.exe";
 done</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>cut basic</t>
+  </si>
+  <si>
+    <t>* cut can accept data passed from pipe or as parameter
+    $ cat abc.txt | cut -d':' -f1-5
+    $ cut -d' ' -f1-5 abc.txt
+* cut fix length 
+    $ cut -c1-5 file.txt
+    $ cut -c10- file.txt
+* cut by delimiter (1-digit) and select fields with option f
+    $ cut -d':' -f5
+    $ cut -d':' -f2-6</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1448,6 +1465,17 @@
       </c>
       <c r="C40" s="5" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="141.75">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Add bash entry on wc and shasum 2. Add git entry on 2016 trend, worktree and rebase 3. Edit old git entry with new category name
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t>linux</t>
   </si>
@@ -621,6 +621,29 @@
 * cut by delimiter (1-digit) and select fields with option f
     $ cut -d':' -f5
     $ cut -d':' -f2-6</t>
+  </si>
+  <si>
+    <t>wc</t>
+  </si>
+  <si>
+    <t>word count</t>
+  </si>
+  <si>
+    <t>wc is a pipe command, its used to count file's word/line/byte count:
+$ cat file.txt | wc -l  //count by lines
+$ cat file.txt | wc -m //count by char
+$ cat file.txt | wc -c //count by bytes</t>
+  </si>
+  <si>
+    <t>sha*sum</t>
+  </si>
+  <si>
+    <t>shasum x sha1sum</t>
+  </si>
+  <si>
+    <t>Command shasum is the extense version of sha1sum. Use below shasum syntax to perform sha1sum:
+$ shasum -a 1 {file}
+$ shasum -a 512 {file}   // perform SHA512 algorithm</t>
   </si>
 </sst>
 </file>
@@ -1014,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1476,6 +1499,28 @@
       </c>
       <c r="C41" s="5" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="78.75">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="63">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry on Jmeter sample, Add bash entry on curl
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="110">
   <si>
     <t>linux</t>
   </si>
@@ -644,6 +644,15 @@
     <t>Command shasum is the extense version of sha1sum. Use below shasum syntax to perform sha1sum:
 $ shasum -a 1 {file}
 $ shasum -a 512 {file}   // perform SHA512 algorithm</t>
+  </si>
+  <si>
+    <t>curl</t>
+  </si>
+  <si>
+    <t>basic curl</t>
+  </si>
+  <si>
+    <t>$ curl 127.0.0.1:8080/date-dummy   //use default GET for url</t>
   </si>
 </sst>
 </file>
@@ -1037,16 +1046,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="30.625" customWidth="1"/>
     <col min="3" max="3" width="56.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1127,7 +1136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="26.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1521,6 +1530,17 @@
       </c>
       <c r="C43" s="5" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add different bash entry and index entry that I learn when updating elyn's website
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
   <si>
     <t>linux</t>
   </si>
@@ -494,7 +494,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -504,7 +504,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -519,7 +519,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -529,7 +529,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -654,16 +654,127 @@
   <si>
     <t>$ curl 127.0.0.1:8080/date-dummy   //use default GET for url</t>
   </si>
+  <si>
+    <t>Check ssh fail atttemp on host</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">$ grep sshd.*Failed /var/log/auth.log      //not only ssh login attemps, sudo attemp and other authoritzation related log </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adduser</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adduser to host</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ adduser new_user_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update public key of a host</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update file: ~/.ssh/known_hosts
+* if a public key from a known host is updated, simply delete the old known_host entry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hydra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to use hydra to crack a ssh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fcrackzip</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intro</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fcrackzip is an util to crack encrypted zip file. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Use nmap to find out whether ssh is on host and the possible username: $nmap -sS -A ip_address
+2. Prepare a wordlist.txt (potential password) support the atk
+3. Use THC-hydra the tool to hack the target ssh: $ hydra -user {username} -list {path_to_wordlist} {target_ip} ssh
+ref: youtube/chris haralson: How to crack an SSH password</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ ssh -v myles@hostname //v for verbose</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linux</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trouble-shoot "Connection reset by xxx.xxx.xxx.xxx" after a certain idle time at client side</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ncrack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ncrack is an sibling project of nmap as another cracking tool like hydra, but it seems not working well when I try to apply it on my linode sshd (no login attemp when check auth.log on host)
+$ ncrack --user myles {target_ip}:{port}
+source code on github.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ref: https://www.bjornjohansen.no/ssh-timeout
+A. PREVENT SSH TIMEOUT ON THE CLIENT SIDE
+Edit your local SSH config file in ~/.ssh/config and add the following line:
+` ServerAliveInterval 120
+(This will send a “null packet” every 120 seconds on your SSH connections to keep them alive.)
+B. PREVENT SSH TIMEOUT ON THE SERVER SIDE
+If you’re a server admin, you can add the following to your SSH daemon config in /etc/ssh/sshd_config on your servers to prevent the clients to time out – so they don’t have to modify their local SSH config:
+` ClientAliveInterval 120
+` ClientAliveCountMax 720
+This will make the server send the clients a “null packet” every 120 seconds and not disconnect them until the client have been inactive for 720 intervals (120 seconds * 720 = 86400 seconds = 24 hours).</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup Hosts and its benefic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup hosts in file /etc/hosts. So that when in ping or ssh or other util, you can use the host alias directly like: $ ssh myles@myleslinode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -674,7 +785,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -696,7 +807,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -749,7 +860,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -762,7 +873,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,6 +947,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -870,6 +982,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1045,21 +1158,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="30.625" customWidth="1"/>
-    <col min="3" max="3" width="56.375" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="72.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1070,7 +1183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25">
+    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1194,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1092,7 +1205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1114,7 +1227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.5">
+    <row r="6" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1238,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="51.75">
+    <row r="7" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1271,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5">
+    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1282,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="93">
+    <row r="11" spans="1:3" ht="94.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1293,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1224,7 +1337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1235,7 +1348,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1246,7 +1359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26.25">
+    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1257,7 +1370,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27">
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1381,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1279,7 +1392,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1290,7 +1403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="26.25">
+    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1301,7 +1414,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="26.25">
+    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1312,7 +1425,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="26.25">
+    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1323,7 +1436,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="26.25">
+    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1334,7 +1447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="39">
+    <row r="26" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -1345,7 +1458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1356,7 +1469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25">
+    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -1367,7 +1480,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
@@ -1378,7 +1491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="51.75">
+    <row r="30" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -1389,7 +1502,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.5">
+    <row r="31" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1400,7 +1513,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1411,7 +1524,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="94.5">
+    <row r="33" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -1422,7 +1535,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="94.5">
+    <row r="34" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1433,7 +1546,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="63">
+    <row r="35" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1444,7 +1557,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="173.25">
+    <row r="36" spans="1:3" ht="178.2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1455,7 +1568,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="63">
+    <row r="37" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1466,7 +1579,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="47.25">
+    <row r="38" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1477,7 +1590,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1488,7 +1601,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="47.25">
+    <row r="40" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -1499,7 +1612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="141.75">
+    <row r="41" spans="1:3" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -1510,7 +1623,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="78.75">
+    <row r="42" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -1521,7 +1634,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="63">
+    <row r="43" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -1532,7 +1645,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -1541,6 +1654,105 @@
       </c>
       <c r="C44" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="81" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1551,12 +1763,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1564,12 +1776,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add bash entry on how to sudo last command
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="136">
   <si>
     <t>linux</t>
   </si>
@@ -494,7 +494,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -504,7 +504,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -519,7 +519,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -529,7 +529,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -765,16 +765,25 @@
     <t>Setup hosts in file /etc/hosts. So that when in ping or ssh or other util, you can use the host alias directly like: $ ssh myles@myleslinode</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>last command</t>
+  </si>
+  <si>
+    <t># 3 ways to find command history
+* sudo !! (aka the fuck)
+* fc -l -10
+* history</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -785,7 +794,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -807,7 +816,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -860,7 +869,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -873,7 +882,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -947,7 +956,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -982,7 +990,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1158,21 +1165,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="72.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="72.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1183,7 +1190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="26.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="40.5">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="51.75">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1267,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1271,7 +1278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1289,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="94.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="93">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1293,7 +1300,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1315,7 +1322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1337,7 +1344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="26.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1377,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="27">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1388,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1414,7 +1421,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="26.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="26.25">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1447,7 +1454,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="39">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -1458,7 +1465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1469,7 +1476,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -1480,7 +1487,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="51.75">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="31.5">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="94.5">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -1535,7 +1542,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="94.5">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1546,7 +1553,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="47.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1557,7 +1564,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="178.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="173.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1568,7 +1575,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="63">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="47.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1601,7 +1608,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="47.25">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -1612,7 +1619,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="141.75">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="63">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -1634,7 +1641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="63">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -1656,7 +1663,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="31.5">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="47.25">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -1689,7 +1696,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="94.5">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -1700,7 +1707,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -1711,7 +1718,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="252">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -1733,7 +1740,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="81" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="78.75">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="31.5">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -1753,6 +1760,17 @@
       </c>
       <c r="C53" s="5" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="63">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1763,12 +1781,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1776,12 +1794,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add python and linux entries
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="154">
   <si>
     <t>linux</t>
   </si>
@@ -494,7 +494,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -504,7 +504,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -519,7 +519,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -529,7 +529,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -543,7 +543,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -553,7 +553,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -774,16 +774,160 @@
 * fc -l -10
 * history</t>
   </si>
+  <si>
+    <t>apt-get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source management</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># Config of apt-get
+There is config file of source provider address: /etc/apt/source.list, you can add your address if you are sure that the software you want to donwload is not available in public standard mirror. 
+# Unmet Error
+It is possible that adding new source address to this config file will cause **unmet** error when installing packages. This error message is like: Install xxx : Depends libxxx (version xxx) but version xxx is to be installed. To solve this problem, remove source address that caused error and run below statement to resume:
+* apt-get clean
+* apt-get autoclean
+* apt-get update</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rfkill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># What is rfkill
+RF-kill is like an software level hardware switch. Say switch on/off the bluetooth/wireless service or others.
+# Basic command
+` sudo rfkill list all`
+` sudo rfkill unblock all`</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lspci</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List PCI Hardware</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># What is lspci
+List PCI command list all hardware that is detected on PCI at hardware level (which means a hardware that appeared on lspci doesn’t mean it's driver is installed and can perform)
+# Common usage
+` lspci | grep -I network`  //show the network card
+` lspci | grep -I ethernet`  //show the ethernet port</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A 輸入法 framework</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t># What is ibus
+IBUS is a 輸入法 framework, it support chinese 倉頡, but make sure the system language installs chinese tradition at the first hand. Its on ubuntu but so far I only use the GUI of ibus. Ctrl-space to turn on an input method.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tarball</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>patch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concept</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Practice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Basic flow
+* Download tarball: `wget {url} `
+* Extract to /usr/local/src: `cd /usr/local/src; tar -zxvf ntp1.0.0.tar.gz`
+* Config the make file: `cd ntp1.0.0/; ./configure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--prefix=/usr/local/ntp`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+* Make: `make clean; make; make check; make install`
+* Link bin: can choose to build soft to /usr/local/bin or to add XXX_HOME and export XXX_HOME/bin to $PATH
+* Link man: do something to MANPATH
+# The Problem of arrangement
+Consider a plan that set standard to install, bin putting and uninstall. If install without a clear domain, then its almost not possible to uninstall it later.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># How to upgrade software wo patch
+In the old tarball, use make to uninstall. Then download the new tarball, configure and make again. And still there can be a miss configure between 2 version (like when making the newer version, you forget to set some old setting)
+# How patch help the upgrade
+Use patch to update the source code, so that you dont need to configure the makefile again (keep the old config), but still need to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>make</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> again or the software binaries will still not be updated/</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -794,7 +938,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -816,8 +960,16 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -869,7 +1021,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -882,7 +1034,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -956,6 +1108,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -990,6 +1143,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1165,21 +1319,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="30.625" customWidth="1"/>
-    <col min="3" max="3" width="72.75" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="72.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1190,7 +1344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25">
+    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1355,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.5">
+    <row r="6" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1245,7 +1399,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="51.75">
+    <row r="7" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1410,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1278,7 +1432,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5">
+    <row r="10" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1289,7 +1443,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="93">
+    <row r="11" spans="1:3" ht="94.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1322,7 +1476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1487,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1344,7 +1498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1355,7 +1509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1366,7 +1520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26.25">
+    <row r="18" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1377,7 +1531,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="27">
+    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1399,7 +1553,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1410,7 +1564,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="26.25">
+    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1421,7 +1575,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="26.25">
+    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1432,7 +1586,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="26.25">
+    <row r="24" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1443,7 +1597,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="26.25">
+    <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
@@ -1454,7 +1608,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="39">
+    <row r="26" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
@@ -1465,7 +1619,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -1476,7 +1630,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25">
+    <row r="28" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -1487,7 +1641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
@@ -1498,7 +1652,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="51.75">
+    <row r="30" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -1509,7 +1663,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.5">
+    <row r="31" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1520,7 +1674,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1531,7 +1685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="94.5">
+    <row r="33" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -1542,7 +1696,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="94.5">
+    <row r="34" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -1553,7 +1707,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25">
+    <row r="35" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1564,7 +1718,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="173.25">
+    <row r="36" spans="1:3" ht="178.2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -1575,7 +1729,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="63">
+    <row r="37" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1586,7 +1740,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="47.25">
+    <row r="38" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1597,7 +1751,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -1608,7 +1762,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="47.25">
+    <row r="40" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -1619,7 +1773,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="141.75">
+    <row r="41" spans="1:3" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -1630,7 +1784,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="63">
+    <row r="42" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -1641,7 +1795,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="63">
+    <row r="43" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -1652,7 +1806,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -1663,7 +1817,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="31.5">
+    <row r="45" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -1674,7 +1828,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -1685,7 +1839,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="47.25">
+    <row r="47" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -1696,7 +1850,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="94.5">
+    <row r="48" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -1707,7 +1861,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -1718,7 +1872,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -1729,7 +1883,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="252">
+    <row r="51" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -1740,7 +1894,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="78.75">
+    <row r="52" spans="1:3" ht="81" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -1751,7 +1905,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="31.5">
+    <row r="53" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -1762,7 +1916,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="63">
+    <row r="54" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1771,6 +1925,72 @@
       </c>
       <c r="C54" s="5" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="194.4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="113.4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="178.2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1781,12 +2001,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1794,12 +2014,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add bash entry on tar x zip options
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
   <si>
     <t>linux</t>
   </si>
@@ -773,6 +773,23 @@
 * sudo !! (aka the fuck)
 * fc -l -10
 * history</t>
+  </si>
+  <si>
+    <t>tar</t>
+  </si>
+  <si>
+    <t># Advance option</t>
+  </si>
+  <si>
+    <t># Zip otpion
+Use z in option to switch on the zip feature: `tar -czvf foo.tar.gz bar/`
+&gt; the f option must place before the file name!
+# Ignore certain folder
+`tar --exclude='.git' --exclude='target/' -czvf foo.tar.gz bar/`
+&gt; Make sure the exclude declare first
+&gt; This will exclude folder in that name among all levels of directory
+# Ignore version controls
+`tar --exclude-vcs ...`</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1771,6 +1788,17 @@
       </c>
       <c r="C54" s="5" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="141.75">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the lost entry back to bash lib
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
   <si>
     <t>linux</t>
   </si>
@@ -94,31 +94,31 @@
   </si>
   <si>
     <t>install git</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>apt-get install git-all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>install unity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>apt-get install ubuntu-desktop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>apt-get install vnc4server</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>vncsever</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -181,30 +181,30 @@
       </rPr>
       <t>-v verbolsely state process</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>variable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1. nano a *.sh file
 2. insert header #!/bin/bash and your command below
 3. chmod +x *.sh
 4. $./*.sh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$sudo chmod u+w {target_file}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$sudo rm -R {target_folder}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>create link</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -237,76 +237,76 @@
       </rPr>
       <t>的意思, -v是有什麼講出來的意思</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Stop job</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Netcat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>check a port</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>send udp package</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>open a listen port</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>scan ports</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>nc -v 127.0.0.1 8080</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>tcp: nc -vnz -w 1 192.168.233.208 1-1000 2000-3000
 udp: nc -vnzu 192.168.1.8 1-65535</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>response in port</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>client: echo "request for anything" | nc 127.0.0.1 5000
 server: nc -l 127.0.0.1 5000 &lt; response.html</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>response in port w HTTP protocol</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>client: [browser]&gt;http://139.162.20.124:9000/
 client: echo -ne "GET / HTTP/1.0\r\n\r\n" | nc 127.0.0.1 9000
 server: while true; do nc -l 9000 &lt; response.html; done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Send HTTP request</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>echo -ne "GET / HTTP/1.0\r\n\r\n" | nc www.google.com 80</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$md5sum -b {filename}
 $sha1sum -b {filename}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -347,40 +347,40 @@
       </rPr>
       <t xml:space="preserve"> echo $MAVEN_HOME</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Ctrl + C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>/*set*/ JAVA_HOME=~/jdk
 /*export*/ export JAVA_HOME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>setup env variable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">In linux, there is a script call .bashrc in your ~ directory that run on your boot. You can export your env variable in this script. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>check cpu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>cat /proc/cpuinfo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>udp: echo "foobar" | nc -u -w1 localhost 5000
@@ -444,7 +444,7 @@
       </rPr>
       <t>p.s. default search into sub-directories.</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Generic</t>
@@ -656,89 +656,89 @@
   </si>
   <si>
     <t>Check ssh fail atttemp on host</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">$ grep sshd.*Failed /var/log/auth.log      //not only ssh login attemps, sudo attemp and other authoritzation related log </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Adduser</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Adduser to host</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$ adduser new_user_name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Update public key of a host</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Update file: ~/.ssh/known_hosts
 * if a public key from a known host is updated, simply delete the old known_host entry</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>hydra</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>How to use hydra to crack a ssh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>fcrackzip</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Intro</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">fcrackzip is an util to crack encrypted zip file. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1. Use nmap to find out whether ssh is on host and the possible username: $nmap -sS -A ip_address
 2. Prepare a wordlist.txt (potential password) support the atk
 3. Use THC-hydra the tool to hack the target ssh: $ hydra -user {username} -list {path_to_wordlist} {target_ip} ssh
 ref: youtube/chris haralson: How to crack an SSH password</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ssh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Basic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>$ ssh -v myles@hostname //v for verbose</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Trouble-shoot "Connection reset by xxx.xxx.xxx.xxx" after a certain idle time at client side</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ncrack</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Ncrack is an sibling project of nmap as another cracking tool like hydra, but it seems not working well when I try to apply it on my linode sshd (no login attemp when check auth.log on host)
 $ ncrack --user myles {target_ip}:{port}
 source code on github.com</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ref: https://www.bjornjohansen.no/ssh-timeout
@@ -751,19 +751,19 @@
 ` ClientAliveInterval 120
 ` ClientAliveCountMax 720
 This will make the server send the clients a “null packet” every 120 seconds and not disconnect them until the client have been inactive for 720 intervals (120 seconds * 720 = 86400 seconds = 24 hours).</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>linux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Setup Hosts and its benefic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Setup hosts in file /etc/hosts. So that when in ping or ssh or other util, you can use the host alias directly like: $ ssh myles@myleslinode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>last command</t>
@@ -791,14 +791,147 @@
 # Ignore version controls
 `tar --exclude-vcs ...`</t>
   </si>
+  <si>
+    <t>apt-get</t>
+  </si>
+  <si>
+    <t>Source management</t>
+  </si>
+  <si>
+    <t># Config of apt-get
+There is config file of source provider address: /etc/apt/source.list, you can add your address if you are sure that the software you want to donwload is not available in public standard mirror. 
+# Unmet Error
+It is possible that adding new source address to this config file will cause **unmet** error when installing packages. This error message is like: Install xxx : Depends libxxx (version xxx) but version xxx is to be installed. To solve this problem, remove source address that caused error and run below statement to resume:
+* apt-get clean
+* apt-get autoclean
+* apt-get update</t>
+  </si>
+  <si>
+    <t>rfkill</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t># What is rfkill
+RF-kill is like an software level hardware switch. Say switch on/off the bluetooth/wireless service or others.
+# Basic command
+` sudo rfkill list all`
+` sudo rfkill unblock all`</t>
+  </si>
+  <si>
+    <t>lspci</t>
+  </si>
+  <si>
+    <t>List PCI Hardware</t>
+  </si>
+  <si>
+    <t># What is lspci
+List PCI command list all hardware that is detected on PCI at hardware level (which means a hardware that appeared on lspci doesn’t mean it's driver is installed and can perform)
+# Common usage
+` lspci | grep -I network`  //show the network card
+` lspci | grep -I ethernet`  //show the ethernet port</t>
+  </si>
+  <si>
+    <t>ibus</t>
+  </si>
+  <si>
+    <t>A 輸入法 framework</t>
+  </si>
+  <si>
+    <t># What is ibus
+IBUS is a 輸入法 framework, it support chinese 倉頡, but make sure the system language installs chinese tradition at the first hand. Its on ubuntu but so far I only use the GUI of ibus. Ctrl-space to turn on an input method.</t>
+  </si>
+  <si>
+    <t>tarball</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Basic flow
+* Download tarball: `wget {url} `
+* Extract to /usr/local/src: `cd /usr/local/src; tar -zxvf ntp1.0.0.tar.gz`
+* Config the make file: `cd ntp1.0.0/; ./configure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--prefix=/usr/local/ntp`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+* Make: `make clean; make; make check; make install`
+* Link bin: can choose to build soft to /usr/local/bin or to add XXX_HOME and export XXX_HOME/bin to $PATH
+* Link man: do something to MANPATH
+# The Problem of arrangement
+Consider a plan that set standard to install, bin putting and uninstall. If install without a clear domain, then its almost not possible to uninstall it later.</t>
+    </r>
+  </si>
+  <si>
+    <t>patch</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># How to upgrade software wo patch
+In the old tarball, use make to uninstall. Then download the new tarball, configure and make again. And still there can be a miss configure between 2 version (like when making the newer version, you forget to set some old setting)
+# How patch help the upgrade
+Use patch to update the source code, so that you dont need to configure the makefile again (keep the old config), but still need to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>make</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> again or the software binaries will still not be updated/</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -837,6 +970,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -870,31 +1018,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1183,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1790,19 +1941,85 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="141.75">
-      <c r="A55" t="s">
+    <row r="55" spans="1:3" ht="189">
+      <c r="A55" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="94.5">
+      <c r="A56" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="110.25">
+      <c r="A57" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="63">
+      <c r="A58" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="173.25">
+      <c r="A59" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="126">
+      <c r="A60" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="141.75">
+      <c r="A61" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B61" t="s">
         <v>137</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1816,7 +2033,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1829,7 +2046,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the bash entry on gpg
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="160">
   <si>
     <t>linux</t>
   </si>
@@ -916,6 +916,28 @@
       </rPr>
       <t xml:space="preserve"> again or the software binaries will still not be updated/</t>
     </r>
+  </si>
+  <si>
+    <t>gpg/ pgp</t>
+  </si>
+  <si>
+    <t># Basic Opts</t>
+  </si>
+  <si>
+    <t># What is pgp/ gpg
+It is an util that implement RSA encryption and decryption methodology
+# Installation
+apt-cyg/ apt-get install gnupg 
+# Operation flow - Create my key-pack and export my public key 
+    * gpg --gen-key  //gpg will ask you a name and it will be regarded as the key id in the local key db
+    * gpg --list-key
+    * gpg --output "myles_public_key.asc" --export "mykey" //"mykey" is the key id in local key databse
+# Operation flow - Decrypt file that is encrypted by others with my public key
+    * gpg --decrypt-files "file_encrypt_with_my_public_key" //gpg will find a key in db that can decrypt
+# Operation flow - Import other's public key and use it to encrypt file 
+    * gpg --import {public_key_from_other.sac}
+    * gpg --list-key  //In here learnt the key id of the newly imported key
+    * gpg --recipient "their_keyid" --output "outputfilename.gpg" --encrypt "file_to_be_encrypted"</t>
   </si>
 </sst>
 </file>
@@ -1334,17 +1356,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.875" customWidth="1"/>
     <col min="2" max="2" width="30.625" customWidth="1"/>
-    <col min="3" max="3" width="72.75" customWidth="1"/>
+    <col min="3" max="3" width="87.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2016,6 +2038,17 @@
       </c>
       <c r="C61" s="5" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="220.5">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ädd bash entry on gpg trust model option
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -937,7 +937,10 @@
 # Operation flow - Import other's public key and use it to encrypt file 
     * gpg --import {public_key_from_other.sac}
     * gpg --list-key  //In here learnt the key id of the newly imported key
-    * gpg --recipient "their_keyid" --output "outputfilename.gpg" --encrypt "file_to_be_encrypted"</t>
+    * gpg --recipient "their_keyid" --output "outputfilename.gpg" --encrypt "file_to_be_encrypted"
+# Issue - trust someone's public key without asking when performing the encryptino
+When gpg encrypt a file with an external public key, it will ask the user to trust it or not, with adding --trust-model always option at the head of the command, it will stop asking for user's validation:
+`gpg --trust-model always --recipient "HKSP" --output e.gpg --encrypt UTF-8-demo.txt`</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1362,7 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C69" sqref="C65:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1765,7 +1768,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="63">
+    <row r="37" spans="1:3" ht="47.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="63">
+    <row r="43" spans="1:3" ht="47.25">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="47.25">
+    <row r="47" spans="1:3" ht="31.5">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="94.5">
+    <row r="48" spans="1:3" ht="78.75">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="252">
+    <row r="51" spans="1:3" ht="204.75">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="78.75">
+    <row r="52" spans="1:3" ht="63">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="189">
+    <row r="55" spans="1:3" ht="173.25">
       <c r="A55" s="6" t="s">
         <v>139</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="110.25">
+    <row r="57" spans="1:3" ht="94.5">
       <c r="A57" s="6" t="s">
         <v>145</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="126">
+    <row r="60" spans="1:3" ht="110.25">
       <c r="A60" s="6" t="s">
         <v>154</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="220.5">
+    <row r="62" spans="1:3" ht="283.5">
       <c r="A62" t="s">
         <v>157</v>
       </c>

</xml_diff>

<commit_message>
Add bash entry on command style: BSD/UNIX/GNU
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>linux</t>
   </si>
@@ -941,6 +941,14 @@
 # Issue - trust someone's public key without asking when performing the encryptino
 When gpg encrypt a file with an external public key, it will ask the user to trust it or not, with adding --trust-model always option at the head of the command, it will stop asking for user's validation:
 `gpg --trust-model always --recipient "HKSP" --output e.gpg --encrypt UTF-8-demo.txt`</t>
+  </si>
+  <si>
+    <t>parameter style</t>
+  </si>
+  <si>
+    <t>ps aux    //this is BSD style
+ps -elf    //this is UNIX Style
+grep --color    //this is GNU style</t>
   </si>
 </sst>
 </file>
@@ -1359,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C69" sqref="C65:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2052,6 +2060,17 @@
       </c>
       <c r="C62" s="5" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="47.25">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tree and watch cmd usage
</commit_message>
<xml_diff>
--- a/bash_lib.xlsx
+++ b/bash_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="168">
   <si>
     <t>linux</t>
   </si>
@@ -949,6 +949,24 @@
     <t>ps aux    //this is BSD style
 ps -elf    //this is UNIX Style
 grep --color    //this is GNU style</t>
+  </si>
+  <si>
+    <t>watch</t>
+  </si>
+  <si>
+    <t>Watch a command repeatly</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>List a directory with selected depth</t>
+  </si>
+  <si>
+    <t>tree -L 2   //list the directory with depth 2</t>
+  </si>
+  <si>
+    <t>watch -n 2 tree    // repeatly update tree command result to stdout by 2 second interval</t>
   </si>
 </sst>
 </file>
@@ -1367,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2071,6 +2089,28 @@
       </c>
       <c r="C63" s="5" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>162</v>
+      </c>
+      <c r="B64" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>